<commit_message>
Cleared all the screenshots and reports
</commit_message>
<xml_diff>
--- a/SalamtekAutomation_v1/TestData/TestData_DEV.xlsx
+++ b/SalamtekAutomation_v1/TestData/TestData_DEV.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5162" uniqueCount="1072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5177" uniqueCount="1073">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -3277,6 +3277,9 @@
   </si>
   <si>
     <t>proForBrand_707</t>
+  </si>
+  <si>
+    <t>proForBrand_259</t>
   </si>
 </sst>
 </file>
@@ -17580,7 +17583,7 @@
         <v>794</v>
       </c>
       <c r="BE21" t="s" s="0">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="BF21" t="s" s="0">
         <v>794</v>

</xml_diff>